<commit_message>
Updated the step analyer file with geometric information
</commit_message>
<xml_diff>
--- a/StepFileAnalyzerFiles/FreeCAD_Circle_stp.xlsx
+++ b/StepFileAnalyzerFiles/FreeCAD_Circle_stp.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16185" windowHeight="8325" tabRatio="700"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="31" r:id="rId1"/>
+    <sheet name="Summary" sheetId="37" r:id="rId1"/>
     <sheet name="Header" sheetId="1" r:id="rId2"/>
     <sheet name="colour_rgb" sheetId="2" r:id="rId3"/>
     <sheet name="curve_style" sheetId="3" r:id="rId4"/>
@@ -39,10 +39,16 @@
     <sheet name="product_definition_context" sheetId="24" r:id="rId25"/>
     <sheet name="product_definition_formation" sheetId="25" r:id="rId26"/>
     <sheet name="product_definition_shape" sheetId="26" r:id="rId27"/>
-    <sheet name="length_unit_and_si_unit" sheetId="27" r:id="rId28"/>
-    <sheet name="plane_angle_unit_and_si_unit" sheetId="28" r:id="rId29"/>
-    <sheet name="si_unit_and_solid_angle_unit" sheetId="29" r:id="rId30"/>
-    <sheet name="uncertainty_measure_with_unit" sheetId="30" r:id="rId31"/>
+    <sheet name="axis2_placement_3d" sheetId="27" r:id="rId28"/>
+    <sheet name="cartesian_point" sheetId="28" r:id="rId29"/>
+    <sheet name="circle" sheetId="29" r:id="rId30"/>
+    <sheet name="direction" sheetId="30" r:id="rId31"/>
+    <sheet name="geometric_curve_set" sheetId="31" r:id="rId32"/>
+    <sheet name="trimmed_curve" sheetId="32" r:id="rId33"/>
+    <sheet name="length_unit_and_si_unit" sheetId="33" r:id="rId34"/>
+    <sheet name="plane_angle_unit_and_si_unit" sheetId="34" r:id="rId35"/>
+    <sheet name="si_unit_and_solid_angle_unit" sheetId="35" r:id="rId36"/>
+    <sheet name="uncertainty_measure_with_unit" sheetId="36" r:id="rId37"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -54,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="276">
   <si>
     <t>Name</t>
   </si>
@@ -245,12 +251,21 @@
     <t>(1) (length_unit) (si_unit) 20   (1) (plane_angle_unit) (si_unit) 21   (1) (si_unit) (solid_angle_unit) 22</t>
   </si>
   <si>
+    <t>(1) shape_representation.context_of_items 10</t>
+  </si>
+  <si>
+    <t>Used In</t>
+  </si>
+  <si>
     <t>(1) uncertainty_measure_with_unit 39</t>
   </si>
   <si>
     <t>(1) (length_unit) (si_unit) 36   (1) (plane_angle_unit) (si_unit) 37   (1) (si_unit) (solid_angle_unit) 38</t>
   </si>
   <si>
+    <t>(1) geometrically_bounded_wireframe_shape_representation.context_of_items 25</t>
+  </si>
+  <si>
     <t>items</t>
   </si>
   <si>
@@ -263,6 +278,15 @@
     <t>(geometric_representation_context) (global_uncertainty_assigned_context) (global_unit_assigned_context) 35</t>
   </si>
   <si>
+    <t>(1) shape_representation 10</t>
+  </si>
+  <si>
+    <t>INV-rep_2</t>
+  </si>
+  <si>
+    <t>(1) shape_definition_representation.used_representation 40</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
@@ -299,6 +323,9 @@
     <t>item_defined_transformation 49</t>
   </si>
   <si>
+    <t>(1) context_dependent_shape_representation.representation_relation 47</t>
+  </si>
+  <si>
     <t>definition</t>
   </si>
   <si>
@@ -317,12 +344,24 @@
     <t>(geometric_representation_context) (global_uncertainty_assigned_context) (global_unit_assigned_context) 19</t>
   </si>
   <si>
+    <t>(1) shape_definition_representation.used_representation 3</t>
+  </si>
+  <si>
+    <t>(1) geometrically_bounded_wireframe_shape_representation 25</t>
+  </si>
+  <si>
+    <t>INV-rep_1</t>
+  </si>
+  <si>
     <t>application</t>
   </si>
   <si>
     <t>core data for automotive mechanical design processes</t>
   </si>
   <si>
+    <t>(2) product_definition_context.frame_of_reference 9 46</t>
+  </si>
+  <si>
     <t>status</t>
   </si>
   <si>
@@ -365,6 +404,9 @@
     <t>reference_designator</t>
   </si>
   <si>
+    <t>(1) product_definition_shape.definition 50</t>
+  </si>
+  <si>
     <t>design</t>
   </si>
   <si>
@@ -380,27 +422,63 @@
     <t>product_definition_context 9</t>
   </si>
   <si>
+    <t>(1) product_definition 42</t>
+  </si>
+  <si>
+    <t>INV-related_product_definition</t>
+  </si>
+  <si>
+    <t>(1) product_definition_shape.definition 4</t>
+  </si>
+  <si>
     <t>product_definition_formation 43</t>
   </si>
   <si>
     <t>product_definition_context 46</t>
   </si>
   <si>
+    <t>(1) product_definition 5</t>
+  </si>
+  <si>
+    <t>INV-relating_product_definition</t>
+  </si>
+  <si>
+    <t>(1) product_definition_shape.definition 41</t>
+  </si>
+  <si>
     <t>part definition</t>
   </si>
   <si>
     <t>life_cycle_stage</t>
   </si>
   <si>
+    <t>(1) product_definition.frame_of_reference 5</t>
+  </si>
+  <si>
+    <t>(1) product_definition.frame_of_reference 42</t>
+  </si>
+  <si>
     <t>of_product</t>
   </si>
   <si>
     <t>product 7</t>
   </si>
   <si>
+    <t>(1) product_definition.formation 5</t>
+  </si>
+  <si>
     <t>product 44</t>
   </si>
   <si>
+    <t>(1) product_definition.formation 42</t>
+  </si>
+  <si>
+    <t>(1) shape_definition_representation.definition 3</t>
+  </si>
+  <si>
+    <t>(1) shape_definition_representation.definition 40</t>
+  </si>
+  <si>
     <t>Placement</t>
   </si>
   <si>
@@ -408,6 +486,111 @@
   </si>
   <si>
     <t>next_assembly_usage_occurrence 51</t>
+  </si>
+  <si>
+    <t>(1) context_dependent_shape_representation.represented_product_relation 47</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>cartesian_point 12</t>
+  </si>
+  <si>
+    <t>axis</t>
+  </si>
+  <si>
+    <t>direction 13</t>
+  </si>
+  <si>
+    <t>ref_direction</t>
+  </si>
+  <si>
+    <t>direction 14</t>
+  </si>
+  <si>
+    <t>cartesian_point 16</t>
+  </si>
+  <si>
+    <t>direction 17</t>
+  </si>
+  <si>
+    <t>direction 18</t>
+  </si>
+  <si>
+    <t>cartesian_point 30</t>
+  </si>
+  <si>
+    <t>direction 31</t>
+  </si>
+  <si>
+    <t>direction 32</t>
+  </si>
+  <si>
+    <t>coordinates</t>
+  </si>
+  <si>
+    <t>0.0 0.0 0.0</t>
+  </si>
+  <si>
+    <t>10.0 0.0 0.0</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>axis2_placement_3d 29</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>direction_ratios</t>
+  </si>
+  <si>
+    <t>0.0 0.0 1.0</t>
+  </si>
+  <si>
+    <t>1.0 0.0 -0.0</t>
+  </si>
+  <si>
+    <t>1.0 0.0 0.0</t>
+  </si>
+  <si>
+    <t>elements</t>
+  </si>
+  <si>
+    <t>(1) trimmed_curve 27</t>
+  </si>
+  <si>
+    <t>basis_curve</t>
+  </si>
+  <si>
+    <t>circle 28</t>
+  </si>
+  <si>
+    <t>trim_1</t>
+  </si>
+  <si>
+    <t>0.0  (1) cartesian_point 33</t>
+  </si>
+  <si>
+    <t>trim_2</t>
+  </si>
+  <si>
+    <t>6.28318530718  (1) cartesian_point 34</t>
+  </si>
+  <si>
+    <t>sense_agreement</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>master_representation</t>
+  </si>
+  <si>
+    <t>parameter</t>
   </si>
   <si>
     <t>dimensions</t>
@@ -530,6 +713,24 @@
     <t>product_definition_shape</t>
   </si>
   <si>
+    <t>axis2_placement_3d</t>
+  </si>
+  <si>
+    <t>cartesian_point</t>
+  </si>
+  <si>
+    <t>circle</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>geometric_curve_set</t>
+  </si>
+  <si>
+    <t>trimmed_curve</t>
+  </si>
+  <si>
     <t>(length_unit)
    (si_unit)</t>
   </si>
@@ -545,34 +746,16 @@
     <t>uncertainty_measure_with_unit</t>
   </si>
   <si>
-    <t>Entity types not processed (7)</t>
-  </si>
-  <si>
-    <t>axis2_placement_3d</t>
-  </si>
-  <si>
-    <t>cartesian_point</t>
-  </si>
-  <si>
-    <t>circle</t>
-  </si>
-  <si>
-    <t>direction</t>
-  </si>
-  <si>
-    <t>geometric_curve_set</t>
+    <t>Entity types not processed (1)</t>
   </si>
   <si>
     <t>product</t>
   </si>
   <si>
-    <t>trimmed_curve</t>
-  </si>
-  <si>
     <t>Spreadsheet generated by the NIST STEP File Analyzer (v1.86)</t>
   </si>
   <si>
-    <t>Mon Oct 17 14:56:15 PDT 2016</t>
+    <t>Tue Oct 18 11:13:12 PDT 2016</t>
   </si>
   <si>
     <t>Schema</t>
@@ -681,6 +864,24 @@
   </si>
   <si>
     <t>product_definition_shape  (3)</t>
+  </si>
+  <si>
+    <t>axis2_placement_3d  (3)</t>
+  </si>
+  <si>
+    <t>cartesian_point  (5)</t>
+  </si>
+  <si>
+    <t>circle  (1)</t>
+  </si>
+  <si>
+    <t>direction  (6)</t>
+  </si>
+  <si>
+    <t>geometric_curve_set  (1)</t>
+  </si>
+  <si>
+    <t>trimmed_curve  (1)</t>
   </si>
   <si>
     <t>(length_unit)(si_unit)  (2)</t>
@@ -732,7 +933,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -759,18 +960,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="50"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="51"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="50"/>
+        <fgColor rgb="FFDDDDFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -818,12 +1031,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -867,14 +1125,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -911,8 +1168,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1252,10 +1527,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>181</v>
+        <v>240</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -1269,10 +1544,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1286,10 +1561,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -1303,7 +1578,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>175</v>
+        <v>234</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>15</v>
@@ -1320,10 +1595,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>173</v>
+        <v>232</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>174</v>
+        <v>233</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -1337,10 +1612,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>171</v>
+        <v>230</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -1355,15 +1630,15 @@
     <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>131</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -1371,7 +1646,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
-        <v>133</v>
+        <v>192</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
@@ -1379,7 +1654,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
-        <v>134</v>
+        <v>193</v>
       </c>
       <c r="B11" s="9">
         <v>1</v>
@@ -1387,7 +1662,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="B12" s="9">
         <v>1</v>
@@ -1395,7 +1670,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
@@ -1403,7 +1678,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
@@ -1411,7 +1686,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
-        <v>138</v>
+        <v>197</v>
       </c>
       <c r="B15" s="9">
         <v>1</v>
@@ -1419,7 +1694,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
@@ -1427,7 +1702,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="19" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
@@ -1435,7 +1710,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="19" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
@@ -1443,7 +1718,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="20" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
@@ -1451,7 +1726,7 @@
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="21" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="B20" s="10">
         <v>2</v>
@@ -1459,7 +1734,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="20" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
@@ -1467,7 +1742,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="20" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
@@ -1475,7 +1750,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
-        <v>146</v>
+        <v>205</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
@@ -1483,7 +1758,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="21" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="B24" s="10">
         <v>1</v>
@@ -1491,7 +1766,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="20" t="s">
-        <v>148</v>
+        <v>207</v>
       </c>
       <c r="B25" s="9">
         <v>2</v>
@@ -1499,7 +1774,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="20" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1507,7 +1782,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="22" t="s">
-        <v>150</v>
+        <v>209</v>
       </c>
       <c r="B27" s="9">
         <v>1</v>
@@ -1515,7 +1790,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="22" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="B28" s="9">
         <v>1</v>
@@ -1523,7 +1798,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="22" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
@@ -1531,7 +1806,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="22" t="s">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c r="B30" s="9">
         <v>2</v>
@@ -1539,7 +1814,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="22" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="B31" s="9">
         <v>2</v>
@@ -1547,7 +1822,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="22" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
       <c r="B32" s="9">
         <v>2</v>
@@ -1555,122 +1830,122 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="22" t="s">
-        <v>156</v>
+        <v>215</v>
       </c>
       <c r="B33" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="B34" s="10">
+        <v>216</v>
+      </c>
+      <c r="B34" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="B35" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B37" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A40" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B40" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="B35" s="10">
+    <row r="41" spans="1:2" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="B41" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="B36" s="10">
+    <row r="42" spans="1:2" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B42" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="B37" s="9">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-    </row>
-    <row r="39" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" s="8"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="B41" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="B42" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-    </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="B44" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="B45" s="9">
-        <v>1</v>
-      </c>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+    </row>
+    <row r="45" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="B46" s="9">
+      <c r="A46" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B46" s="8"/>
+    </row>
+    <row r="47" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B47" s="11">
         <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" s="11">
-        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1711,14 +1986,20 @@
     <hyperlink ref="A31" r:id="rId26" location="product_definition_context!A4" tooltip="Go to product_definition_context" display="FreeCAD_Circle_stp.xlsx - product_definition_context!A4"/>
     <hyperlink ref="A32" r:id="rId27" location="product_definition_formation!A4" tooltip="Go to product_definition_formation" display="FreeCAD_Circle_stp.xlsx - product_definition_formation!A4"/>
     <hyperlink ref="A33" r:id="rId28" location="product_definition_shape!A4" tooltip="Go to product_definition_shape" display="FreeCAD_Circle_stp.xlsx - product_definition_shape!A4"/>
-    <hyperlink ref="A34" r:id="rId29" location="length_unit_and_si_unit!A4" tooltip="Go to length_unit_and_si_unit" display="FreeCAD_Circle_stp.xlsx - length_unit_and_si_unit!A4"/>
-    <hyperlink ref="A35" r:id="rId30" location="plane_angle_unit_and_si_unit!A4" tooltip="Go to plane_angle_unit_and_si_unit" display="FreeCAD_Circle_stp.xlsx - plane_angle_unit_and_si_unit!A4"/>
-    <hyperlink ref="A36" r:id="rId31" location="si_unit_and_solid_angle_unit!A4" tooltip="Go to si_unit_and_solid_angle_unit" display="FreeCAD_Circle_stp.xlsx - si_unit_and_solid_angle_unit!A4"/>
-    <hyperlink ref="A37" r:id="rId32" location="uncertainty_measure_with_unit!A4" tooltip="Go to uncertainty_measure_with_unit" display="FreeCAD_Circle_stp.xlsx - uncertainty_measure_with_unit!A4"/>
+    <hyperlink ref="A34" r:id="rId29" location="axis2_placement_3d!A4" tooltip="Go to axis2_placement_3d" display="FreeCAD_Circle_stp.xlsx - axis2_placement_3d!A4"/>
+    <hyperlink ref="A35" r:id="rId30" location="cartesian_point!A4" tooltip="Go to cartesian_point" display="FreeCAD_Circle_stp.xlsx - cartesian_point!A4"/>
+    <hyperlink ref="A36" r:id="rId31" location="circle!A4" tooltip="Go to circle" display="FreeCAD_Circle_stp.xlsx - circle!A4"/>
+    <hyperlink ref="A37" r:id="rId32" location="direction!A4" tooltip="Go to direction" display="FreeCAD_Circle_stp.xlsx - direction!A4"/>
+    <hyperlink ref="A38" r:id="rId33" location="geometric_curve_set!A4" tooltip="Go to geometric_curve_set" display="FreeCAD_Circle_stp.xlsx - geometric_curve_set!A4"/>
+    <hyperlink ref="A39" r:id="rId34" location="trimmed_curve!A4" tooltip="Go to trimmed_curve" display="FreeCAD_Circle_stp.xlsx - trimmed_curve!A4"/>
+    <hyperlink ref="A40" r:id="rId35" location="length_unit_and_si_unit!A4" tooltip="Go to length_unit_and_si_unit" display="FreeCAD_Circle_stp.xlsx - length_unit_and_si_unit!A4"/>
+    <hyperlink ref="A41" r:id="rId36" location="plane_angle_unit_and_si_unit!A4" tooltip="Go to plane_angle_unit_and_si_unit" display="FreeCAD_Circle_stp.xlsx - plane_angle_unit_and_si_unit!A4"/>
+    <hyperlink ref="A42" r:id="rId37" location="si_unit_and_solid_angle_unit!A4" tooltip="Go to si_unit_and_solid_angle_unit" display="FreeCAD_Circle_stp.xlsx - si_unit_and_solid_angle_unit!A4"/>
+    <hyperlink ref="A43" r:id="rId38" location="uncertainty_measure_with_unit!A4" tooltip="Go to uncertainty_measure_with_unit" display="FreeCAD_Circle_stp.xlsx - uncertainty_measure_with_unit!A4"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -1745,37 +2026,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>57</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1784,7 +2065,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1812,31 +2093,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>58</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1845,7 +2126,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1874,37 +2155,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>56</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1913,7 +2194,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1936,43 +2217,43 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="71.1328125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="71.1328125" style="35" customWidth="1"/>
     <col min="3" max="3" width="25.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>47</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1981,7 +2262,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2001,88 +2282,98 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.3984375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.796875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.19921875" style="36" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="6"/>
+    <col min="6" max="6" width="71.19921875" style="35" customWidth="1"/>
+    <col min="7" max="7" width="66.6640625" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="36" t="s">
         <v>61</v>
       </c>
+      <c r="G3" s="42" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>19</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="38">
         <v>3</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="43" t="s">
         <v>62</v>
       </c>
+      <c r="G4" s="40" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>35</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>64</v>
+      <c r="E5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2090,7 +2381,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2110,54 +2401,68 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="45.53125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.19921875" style="36" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="4" max="4" width="71.19921875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="23.19921875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="48.796875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>67</v>
+      <c r="C3" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>25</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>68</v>
+      <c r="C4" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2165,7 +2470,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2195,50 +2500,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>72</v>
+      <c r="C3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>49</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>73</v>
+      <c r="D4" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2246,7 +2551,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2271,49 +2576,49 @@
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="15.1328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.19921875" style="36" customWidth="1"/>
+    <col min="4" max="4" width="71.19921875" style="35" customWidth="1"/>
     <col min="5" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>67</v>
+      <c r="C3" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>53</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>68</v>
+      <c r="C4" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2321,7 +2626,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2341,7 +2646,7 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
@@ -2349,60 +2654,67 @@
     <col min="4" max="4" width="49.53125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.46484375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="6"/>
+    <col min="7" max="7" width="59.19921875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>79</v>
+      <c r="D3" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>48</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>80</v>
+      <c r="D4" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2410,7 +2722,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2439,49 +2751,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>83</v>
+      <c r="B3" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>3</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="28">
+        <v>40</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>82</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
-        <v>40</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2489,7 +2801,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2616,54 +2928,68 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.19921875" style="36" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="4" max="4" width="71.19921875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="47.796875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="52.19921875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>67</v>
+      <c r="C3" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>10</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>86</v>
+      <c r="C4" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +2997,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2691,40 +3017,47 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.46484375" style="6" customWidth="1"/>
     <col min="2" max="2" width="43.796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="6"/>
+    <col min="3" max="3" width="45.53125" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>87</v>
+      <c r="B3" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>88</v>
+      <c r="B4" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2732,7 +3065,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2763,50 +3096,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>87</v>
+      <c r="B3" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="29">
+      <c r="B4" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="28">
         <v>1997</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>94</v>
+      <c r="E4" s="28" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2814,7 +3147,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2834,7 +3167,7 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="2.265625" style="7" customWidth="1"/>
@@ -2843,66 +3176,73 @@
     <col min="5" max="5" width="23.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.9296875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="6"/>
+    <col min="8" max="8" width="34.53125" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>102</v>
+      <c r="D3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>51</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="30" t="s">
+      <c r="B4" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="30" t="s">
+      <c r="E4" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="29" t="s">
         <v>13</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2910,7 +3250,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2930,78 +3270,104 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="5.796875" style="7" customWidth="1"/>
     <col min="3" max="3" width="9.86328125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.9296875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.06640625" style="6"/>
+    <col min="6" max="6" width="26.53125" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="34.53125" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="26.9296875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="32" t="s">
+      <c r="B3" s="32" t="s">
         <v>106</v>
       </c>
+      <c r="C3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>5</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="40" t="s">
+      <c r="B4" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>107</v>
-      </c>
+      <c r="D4" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>42</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>109</v>
+      <c r="D5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3009,7 +3375,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3029,68 +3395,78 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="12.06640625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.9296875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.53125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="5" max="5" width="37" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>111</v>
+      <c r="C3" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>9</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>103</v>
+      <c r="B4" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>46</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>103</v>
+      <c r="B5" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3098,7 +3474,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3118,68 +3494,78 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="2.265625" style="7" customWidth="1"/>
     <col min="3" max="3" width="9.86328125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="5" max="5" width="29.19921875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>112</v>
+      <c r="B3" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>6</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="39" t="s">
-        <v>113</v>
+      <c r="D4" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>43</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>114</v>
+      <c r="D5" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3187,7 +3573,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3207,82 +3593,95 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
     <col min="2" max="2" width="9" style="7" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.1328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="5" max="5" width="64.19921875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>81</v>
+      <c r="C3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="39" t="s">
-        <v>99</v>
+      <c r="D4" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="39">
+      <c r="A5" s="38">
         <v>41</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="39" t="s">
-        <v>101</v>
+      <c r="D5" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>50</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>117</v>
+      <c r="B6" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3290,7 +3689,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3299,9 +3698,9 @@
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor indexed="51"/>
+    <tabColor indexed="50"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -3313,61 +3712,92 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.3984375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="5.46484375" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15.46484375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="32" t="s">
         <v>23</v>
       </c>
+      <c r="C3" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
-        <v>20</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
-        <v>36</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>121</v>
+      <c r="A4" s="38">
+        <v>11</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="38">
+        <v>15</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="28">
+        <v>29</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3375,7 +3805,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3384,9 +3814,9 @@
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor indexed="51"/>
+    <tabColor indexed="50"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -3398,57 +3828,88 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.3984375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="5.73046875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="32" t="s">
         <v>23</v>
       </c>
+      <c r="C3" s="31" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
-        <v>21</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
-        <v>37</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29" t="s">
-        <v>122</v>
+      <c r="A4" s="38">
+        <v>12</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="38">
+        <v>16</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="38">
+        <v>30</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="38">
+        <v>33</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="28">
+        <v>34</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3456,7 +3917,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3485,49 +3946,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>61</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3536,7 +3997,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId2"/>
@@ -3544,6 +4005,534 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor indexed="50"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.46484375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.73046875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="28">
+        <v>28</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="28">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor indexed="50"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="38">
+        <v>13</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="38">
+        <v>14</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="38">
+        <v>17</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="38">
+        <v>18</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="38">
+        <v>31</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="28">
+        <v>32</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor indexed="50"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="28">
+        <v>26</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor indexed="50"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="28">
+        <v>27</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor indexed="51"/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.3984375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="5.46484375" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="38">
+        <v>20</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="28">
+        <v>36</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor indexed="51"/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.3984375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="5.73046875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="38">
+        <v>21</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="28">
+        <v>37</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor indexed="51"/>
@@ -3567,50 +4556,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="32" t="s">
+      <c r="B3" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>22</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39" t="s">
-        <v>123</v>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>38</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29" t="s">
-        <v>123</v>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3618,13 +4607,13 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor indexed="51"/>
@@ -3649,67 +4638,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="33" t="s">
+      <c r="B3" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>69</v>
+      <c r="E3" s="32" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="39">
+      <c r="A4" s="38">
         <v>23</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="47">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>128</v>
+      <c r="C4" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>39</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="48">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>128</v>
+      <c r="C5" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3717,7 +4706,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3748,49 +4737,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>62</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <v>0.1</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="28" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3799,7 +4788,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3827,31 +4816,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>63</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3860,7 +4849,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3889,37 +4878,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>185</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>59</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3928,7 +4917,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3957,37 +4946,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>60</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3996,7 +4985,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4024,31 +5013,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>55</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4057,7 +5046,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4087,43 +5076,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="A1" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>54</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4132,7 +5121,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="Summary!A30" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A30"/>
+    <hyperlink ref="A1" r:id="rId1" location="Summary!A36" tooltip="Return to Summary" display="FreeCAD_Circle_stp.xlsx - Summary!A36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>